<commit_message>
Added further parameters and calculations for the board
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="63">
   <si>
     <t>mm</t>
   </si>
@@ -68,23 +68,6 @@
   </si>
   <si>
     <t>k_poleoff</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Keycap pole offset for alignment </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(calculated)</t>
-    </r>
   </si>
   <si>
     <t>k_cmxw</t>
@@ -180,6 +163,118 @@
   </si>
   <si>
     <t>Keyswitch Pole Base Height</t>
+  </si>
+  <si>
+    <t>Keyboard Dimensions</t>
+  </si>
+  <si>
+    <t>b_pad</t>
+  </si>
+  <si>
+    <t>Padding between keys</t>
+  </si>
+  <si>
+    <t>b_tab</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>b_caps</t>
+  </si>
+  <si>
+    <t>b_lshift</t>
+  </si>
+  <si>
+    <t>b_rshift</t>
+  </si>
+  <si>
+    <t>b_ctrl</t>
+  </si>
+  <si>
+    <t>b_space</t>
+  </si>
+  <si>
+    <t>Key Multipliers</t>
+  </si>
+  <si>
+    <t>Tab, \</t>
+  </si>
+  <si>
+    <t>Lshift, Enter</t>
+  </si>
+  <si>
+    <t>Rshift</t>
+  </si>
+  <si>
+    <t>Ctrl, Alt, Win</t>
+  </si>
+  <si>
+    <t>Space</t>
+  </si>
+  <si>
+    <t>Caps</t>
+  </si>
+  <si>
+    <t>Capslock Width</t>
+  </si>
+  <si>
+    <t>Right Shift Width</t>
+  </si>
+  <si>
+    <t>Space Bar Width</t>
+  </si>
+  <si>
+    <t>Tab and Backslash key  width</t>
+  </si>
+  <si>
+    <t>Left Shift  and Enter Width</t>
+  </si>
+  <si>
+    <t>Ctrl, Alt, Win and Menu Keys Width</t>
+  </si>
+  <si>
+    <t>b_width</t>
+  </si>
+  <si>
+    <t>b_height</t>
+  </si>
+  <si>
+    <t>Keyboard Width (including padding)</t>
+  </si>
+  <si>
+    <t>Keyboard Height (including padding)</t>
+  </si>
+  <si>
+    <t>Row 1 - 2 Offset</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Keycap pole offset for alignment </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(calculated) </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Must not be greater than 3</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -283,7 +378,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -373,6 +468,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -381,7 +485,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -401,6 +505,14 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -412,6 +524,25 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -718,10 +849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -731,9 +862,11 @@
     <col min="3" max="3" width="9.140625" style="5"/>
     <col min="4" max="4" width="60.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="28.140625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -746,11 +879,11 @@
       <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E1" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -763,9 +896,14 @@
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="1:5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="11"/>
+      <c r="H2" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+    </row>
+    <row r="3" spans="1:11" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -778,9 +916,18 @@
       <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="7"/>
-    </row>
-    <row r="4" spans="1:5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E3" s="11"/>
+      <c r="H3" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -793,9 +940,18 @@
       <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="1:5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="11"/>
+      <c r="H4" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -808,9 +964,18 @@
       <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="7"/>
-    </row>
-    <row r="6" spans="1:5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="11"/>
+      <c r="H5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" s="3">
+        <v>2.25</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -823,9 +988,18 @@
       <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="7"/>
-    </row>
-    <row r="7" spans="1:5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E6" s="11"/>
+      <c r="H6" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" s="3">
+        <v>2.75</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -838,9 +1012,18 @@
       <c r="D7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="7"/>
-    </row>
-    <row r="8" spans="1:5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="11"/>
+      <c r="H7" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="3">
+        <v>1.25</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -853,26 +1036,38 @@
       <c r="D8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="7"/>
-    </row>
-    <row r="9" spans="1:5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="11"/>
+      <c r="H8" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" s="3">
+        <v>6.5</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="4">
-        <v>2</v>
+        <f>$I$11/2</f>
+        <v>2.2625000000000011</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+    </row>
+    <row r="10" spans="1:11" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="3">
         <v>5.54</v>
@@ -881,13 +1076,13 @@
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="7"/>
-    </row>
-    <row r="11" spans="1:5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="E10" s="11"/>
+    </row>
+    <row r="11" spans="1:11" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="3">
         <v>1.35</v>
@@ -896,13 +1091,24 @@
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="1:5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="G11" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="21"/>
+      <c r="I11" s="10">
+        <f>B19-B18</f>
+        <v>4.5250000000000021</v>
+      </c>
+      <c r="J11" s="19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="3">
         <v>4.4000000000000004</v>
@@ -911,13 +1117,13 @@
         <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="E12" s="11"/>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="3">
         <v>15.6</v>
@@ -926,15 +1132,15 @@
         <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="B14" s="3">
         <v>3.6</v>
@@ -943,13 +1149,13 @@
         <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="13"/>
+    </row>
+    <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="E14" s="9"/>
-    </row>
-    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="B15" s="3">
         <v>5.5</v>
@@ -958,13 +1164,13 @@
         <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="9"/>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="E15" s="13"/>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="3">
         <v>7</v>
@@ -973,14 +1179,162 @@
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="14"/>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="10"/>
+    </row>
+    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="3">
+        <f>I3*$B$1</f>
+        <v>27.150000000000002</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="17"/>
+    </row>
+    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="3">
+        <f t="shared" ref="B19:B23" si="0">I4*$B$1</f>
+        <v>31.675000000000004</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="17"/>
+    </row>
+    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="3">
+        <f t="shared" si="0"/>
+        <v>40.725000000000001</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="17"/>
+    </row>
+    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="3">
+        <f t="shared" si="0"/>
+        <v>49.775000000000006</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="17"/>
+    </row>
+    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="3">
+        <f t="shared" si="0"/>
+        <v>22.625</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="17"/>
+    </row>
+    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="3">
+        <f t="shared" si="0"/>
+        <v>117.65</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="17"/>
+    </row>
+    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="3">
+        <f>$B$17 +2*($B$18+$B$17)+12*($B$1+$B$17)</f>
+        <v>286.5</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E24" s="17"/>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="3">
+        <f>$B$17+4*($B$1+$B$17)</f>
+        <v>77.400000000000006</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="E1:E12"/>
     <mergeCell ref="E13:E16"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="E17:E25"/>
+    <mergeCell ref="G11:H11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added a smaller keycap variant
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="71">
   <si>
     <t>mm</t>
   </si>
@@ -275,6 +275,30 @@
       </rPr>
       <t>Must not be greater than 3</t>
     </r>
+  </si>
+  <si>
+    <t>k_staper</t>
+  </si>
+  <si>
+    <t>k_ltaper</t>
+  </si>
+  <si>
+    <t>Taper Length for smaller keycap, around Left, Top and Right edges</t>
+  </si>
+  <si>
+    <t>Taper Length for larger keycap, around Left, Top and Right edges</t>
+  </si>
+  <si>
+    <t>k_sradius</t>
+  </si>
+  <si>
+    <t>k_lradius</t>
+  </si>
+  <si>
+    <t>Radius for smaller keycap along top edge</t>
+  </si>
+  <si>
+    <t>Radius for larger keycap along top edge</t>
   </si>
 </sst>
 </file>
@@ -485,7 +509,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -512,9 +536,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="4" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -849,10 +870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -860,13 +881,13 @@
     <col min="1" max="1" width="13" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="3"/>
     <col min="3" max="3" width="9.140625" style="5"/>
-    <col min="4" max="4" width="60.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="67.42578125" style="2" customWidth="1"/>
     <col min="5" max="5" width="28.140625" style="6" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" customWidth="1"/>
     <col min="10" max="10" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -879,11 +900,11 @@
       <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:11" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -896,14 +917,14 @@
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="H2" s="15" t="s">
+      <c r="E2" s="16"/>
+      <c r="H2" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-    </row>
-    <row r="3" spans="1:11" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+    </row>
+    <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -916,7 +937,7 @@
       <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="11"/>
+      <c r="E3" s="16"/>
       <c r="H3" s="8" t="s">
         <v>45</v>
       </c>
@@ -927,7 +948,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:11" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -940,7 +961,7 @@
       <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="11"/>
+      <c r="E4" s="16"/>
       <c r="H4" s="8" t="s">
         <v>50</v>
       </c>
@@ -951,20 +972,20 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:11" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="B5" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="11"/>
+        <v>65</v>
+      </c>
+      <c r="E5" s="16"/>
       <c r="H5" s="8" t="s">
         <v>46</v>
       </c>
@@ -975,20 +996,20 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:11" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="B6" s="3">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="11"/>
+        <v>69</v>
+      </c>
+      <c r="E6" s="16"/>
       <c r="H6" s="8" t="s">
         <v>47</v>
       </c>
@@ -999,9 +1020,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:11" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="B7" s="3">
         <v>1.5</v>
@@ -1010,9 +1031,9 @@
         <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="11"/>
+        <v>66</v>
+      </c>
+      <c r="E7" s="16"/>
       <c r="H7" s="8" t="s">
         <v>48</v>
       </c>
@@ -1023,20 +1044,20 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:11" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="B8" s="3">
-        <v>5</v>
+        <v>6.5</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="11"/>
+        <v>70</v>
+      </c>
+      <c r="E8" s="16"/>
       <c r="H8" s="8" t="s">
         <v>49</v>
       </c>
@@ -1047,294 +1068,354 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:11" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="3">
+        <v>6</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+    </row>
+    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="16"/>
+    </row>
+    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="16"/>
+      <c r="G11" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="20"/>
+      <c r="I11" s="10">
+        <f>B23-B22</f>
+        <v>4.5250000000000021</v>
+      </c>
+      <c r="J11" s="18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="3">
+        <v>5</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="16"/>
+    </row>
+    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B13" s="4">
         <f>$I$11/2</f>
         <v>2.2625000000000011</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="C13" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-    </row>
-    <row r="10" spans="1:11" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="3">
-        <v>5.54</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="11"/>
-    </row>
-    <row r="11" spans="1:11" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="3">
-        <v>1.35</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="11"/>
-      <c r="G11" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="H11" s="21"/>
-      <c r="I11" s="10">
-        <f>B19-B18</f>
-        <v>4.5250000000000021</v>
-      </c>
-      <c r="J11" s="19" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="3">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="11"/>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="3">
-        <v>15.6</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>25</v>
-      </c>
+      <c r="E13" s="16"/>
     </row>
     <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B14" s="3">
-        <v>3.6</v>
+        <v>5.54</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="13"/>
+        <v>21</v>
+      </c>
+      <c r="E14" s="16"/>
     </row>
     <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B15" s="3">
-        <v>5.5</v>
+        <v>1.35</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="13"/>
+        <v>19</v>
+      </c>
+      <c r="E15" s="16"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B16" s="3">
-        <v>7</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="14"/>
+        <v>23</v>
+      </c>
+      <c r="E16" s="17"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B17" s="3">
-        <v>1</v>
+        <v>15.6</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>34</v>
+        <v>27</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="3">
+        <v>3.6</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="12"/>
+    </row>
+    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="12"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="3">
+        <v>7</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="13"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="3">
+        <v>1</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B22" s="3">
         <f>I3*$B$1</f>
         <v>27.150000000000002</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D18" s="2" t="s">
+      <c r="C22" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E18" s="17"/>
-    </row>
-    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="3">
-        <f t="shared" ref="B19:B23" si="0">I4*$B$1</f>
-        <v>31.675000000000004</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E19" s="17"/>
-    </row>
-    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="3">
-        <f t="shared" si="0"/>
-        <v>40.725000000000001</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E20" s="17"/>
-    </row>
-    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="3">
-        <f t="shared" si="0"/>
-        <v>49.775000000000006</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E21" s="17"/>
-    </row>
-    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="3">
-        <f t="shared" si="0"/>
-        <v>22.625</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" s="17"/>
+      <c r="E22" s="16"/>
     </row>
     <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B23" s="3">
-        <f t="shared" si="0"/>
-        <v>117.65</v>
+        <f>I4*$B$1</f>
+        <v>31.675000000000004</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E23" s="17"/>
+        <v>51</v>
+      </c>
+      <c r="E23" s="16"/>
     </row>
     <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="3">
+        <f>I5*$B$1</f>
+        <v>40.725000000000001</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" s="16"/>
+    </row>
+    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="3">
+        <f>I6*$B$1</f>
+        <v>49.775000000000006</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" s="16"/>
+    </row>
+    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="3">
+        <f>I7*$B$1</f>
+        <v>22.625</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="16"/>
+    </row>
+    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="3">
+        <f>I8*$B$1</f>
+        <v>117.65</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" s="16"/>
+    </row>
+    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="3">
-        <f>$B$17 +2*($B$18+$B$17)+12*($B$1+$B$17)</f>
+      <c r="B28" s="3">
+        <f>$B$21 +2*($B$22+$B$21)+12*($B$1+$B$21)</f>
         <v>286.5</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="C28" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E24" s="17"/>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+      <c r="E28" s="16"/>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="3">
-        <f>$B$17+4*($B$1+$B$17)</f>
+      <c r="B29" s="3">
+        <f>$B$21+4*($B$1+$B$21)</f>
         <v>77.400000000000006</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D25" s="2" t="s">
+      <c r="C29" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E25" s="18"/>
+      <c r="E29" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="E1:E12"/>
-    <mergeCell ref="E13:E16"/>
+    <mergeCell ref="E17:E20"/>
     <mergeCell ref="H2:J2"/>
-    <mergeCell ref="E17:E25"/>
+    <mergeCell ref="E21:E29"/>
     <mergeCell ref="G11:H11"/>
+    <mergeCell ref="E1:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added larger keycap and placed on keyboard
Reviewing the smaller and larger keycaps, everything seems to fit
properly. Checking my keyboard, there seems to be no collisions with
keyswitches. We may add to the keycap pole to provide raising for the
top rows and relatively lower the thumb keys.

Also color coded some parts to make comparison easier.
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -873,7 +873,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -1048,8 +1048,9 @@
       <c r="A8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="3">
-        <v>6.5</v>
+      <c r="B8" s="4">
+        <f>B9</f>
+        <v>6</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Added a spacebar mockup (for thumb clearance comparison)
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -14,18 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="73">
   <si>
     <t>mm</t>
   </si>
   <si>
-    <t>Taper Length for Front of keycap - where finger goes</t>
-  </si>
-  <si>
     <t>Keycap curve radius for Top edge</t>
-  </si>
-  <si>
-    <t>Taper Length for keycap, around Left, Top and Right edges</t>
   </si>
   <si>
     <t>Keycap Shell width (wall thickness)</t>
@@ -299,6 +293,18 @@
   </si>
   <si>
     <t>Radius for larger keycap along top edge</t>
+  </si>
+  <si>
+    <t>Taper Length for Front of keycap - where finger goes (sides, for thumb keycap)</t>
+  </si>
+  <si>
+    <t>Taper Length for keycap, around Left, Top and Right edges (top and bottom, for thumb keycap)</t>
+  </si>
+  <si>
+    <t>k_height_t</t>
+  </si>
+  <si>
+    <t>Thumb row keycap height</t>
   </si>
 </sst>
 </file>
@@ -537,6 +543,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -558,7 +565,6 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -870,10 +876,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -881,7 +887,7 @@
     <col min="1" max="1" width="13" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="3"/>
     <col min="3" max="3" width="9.140625" style="5"/>
-    <col min="4" max="4" width="67.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="86.85546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="28.140625" style="6" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" customWidth="1"/>
     <col min="10" max="10" width="7.7109375" customWidth="1"/>
@@ -889,7 +895,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="3">
         <v>18.100000000000001</v>
@@ -898,15 +904,15 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>24</v>
+        <v>4</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" s="3">
         <v>15</v>
@@ -915,195 +921,195 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="16"/>
-      <c r="H2" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
+        <v>3</v>
+      </c>
+      <c r="E2" s="17"/>
+      <c r="H2" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
     </row>
     <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
       <c r="B3" s="3">
-        <v>1.5</v>
+        <v>13</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="16"/>
+        <v>72</v>
+      </c>
+      <c r="E3" s="17"/>
       <c r="H3" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I3" s="10">
         <v>1.5</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="16"/>
+        <v>70</v>
+      </c>
+      <c r="E4" s="17"/>
       <c r="H4" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I4" s="3">
         <v>1.75</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="B5" s="3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" s="16"/>
+        <v>69</v>
+      </c>
+      <c r="E5" s="17"/>
       <c r="H5" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I5" s="3">
         <v>2.25</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B6" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E6" s="16"/>
+        <v>63</v>
+      </c>
+      <c r="E6" s="17"/>
       <c r="H6" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I6" s="3">
         <v>2.75</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B7" s="3">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E7" s="16"/>
+        <v>67</v>
+      </c>
+      <c r="E7" s="17"/>
       <c r="H7" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I7" s="3">
         <v>1.25</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="4">
-        <f>B9</f>
-        <v>6</v>
+        <v>62</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1.5</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" s="16"/>
+        <v>64</v>
+      </c>
+      <c r="E8" s="17"/>
       <c r="H8" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I8" s="3">
         <v>6.5</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="3">
+        <v>66</v>
+      </c>
+      <c r="B9" s="4">
+        <f>B10</f>
         <v>6</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="16"/>
+        <v>68</v>
+      </c>
+      <c r="E9" s="17"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
     </row>
     <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3">
-        <v>1.5</v>
+        <v>6</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="16"/>
+        <v>1</v>
+      </c>
+      <c r="E10" s="17"/>
     </row>
     <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3">
         <v>1.5</v>
@@ -1112,73 +1118,73 @@
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="16"/>
+        <v>2</v>
+      </c>
+      <c r="E11" s="17"/>
       <c r="G11" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H11" s="20"/>
       <c r="I11" s="10">
-        <f>B23-B22</f>
+        <f>B24-B23</f>
         <v>4.5250000000000021</v>
       </c>
-      <c r="J11" s="18" t="s">
+      <c r="J11" s="11" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="16"/>
+        <v>12</v>
+      </c>
+      <c r="E12" s="17"/>
     </row>
     <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="4">
+        <v>13</v>
+      </c>
+      <c r="B13" s="3">
+        <v>5</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="17"/>
+    </row>
+    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="4">
         <f>$I$11/2</f>
         <v>2.2625000000000011</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" s="16"/>
-    </row>
-    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="3">
-        <v>5.54</v>
-      </c>
       <c r="C14" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="16"/>
+        <v>60</v>
+      </c>
+      <c r="E14" s="17"/>
     </row>
     <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="3">
-        <v>1.35</v>
+        <v>5.54</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>0</v>
@@ -1186,237 +1192,252 @@
       <c r="D15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="16"/>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E15" s="17"/>
+    </row>
+    <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B16" s="3">
+        <v>1.35</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="17"/>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="3">
         <v>4.4000000000000004</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="2" t="s">
+      <c r="C17" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="18"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="3">
+        <v>15.6</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="17"/>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="3">
-        <v>15.6</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="3">
-        <v>3.6</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" s="12"/>
     </row>
     <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="3">
+        <v>3.6</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="13"/>
+    </row>
+    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="3">
-        <v>5.5</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="2" t="s">
+      <c r="E20" s="13"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="3">
+        <v>7</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="14"/>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="3">
+        <v>1</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="12"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="3">
-        <v>7</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" s="13"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    </row>
+    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="3">
-        <v>1</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="3">
+      <c r="B23" s="3">
         <f>I3*$B$1</f>
         <v>27.150000000000002</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E22" s="16"/>
-    </row>
-    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="3">
+      <c r="C23" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="17"/>
+    </row>
+    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="3">
         <f>I4*$B$1</f>
         <v>31.675000000000004</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E23" s="16"/>
-    </row>
-    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" s="3">
+      <c r="C24" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="17"/>
+    </row>
+    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="3">
         <f>I5*$B$1</f>
         <v>40.725000000000001</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E24" s="16"/>
-    </row>
-    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="3">
+      <c r="C25" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" s="17"/>
+    </row>
+    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="3">
         <f>I6*$B$1</f>
         <v>49.775000000000006</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E25" s="16"/>
-    </row>
-    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" s="3">
+      <c r="C26" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" s="17"/>
+    </row>
+    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="3">
         <f>I7*$B$1</f>
         <v>22.625</v>
       </c>
-      <c r="C26" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E26" s="16"/>
-    </row>
-    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="3">
+      <c r="C27" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E27" s="17"/>
+    </row>
+    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="3">
         <f>I8*$B$1</f>
         <v>117.65</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E27" s="16"/>
-    </row>
-    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="C28" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E28" s="17"/>
+    </row>
+    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="3">
+        <f>$B$22 +2*($B$23+$B$22)+12*($B$1+$B$22)</f>
+        <v>286.5</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="3">
-        <f>$B$21 +2*($B$22+$B$21)+12*($B$1+$B$21)</f>
-        <v>286.5</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E28" s="16"/>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+      <c r="E29" s="17"/>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="3">
+        <f>$B$22+4*($B$1+$B$22)</f>
+        <v>77.400000000000006</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="3">
-        <f>$B$21+4*($B$1+$B$21)</f>
-        <v>77.400000000000006</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E29" s="17"/>
+      <c r="E30" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="E17:E20"/>
+    <mergeCell ref="E18:E21"/>
     <mergeCell ref="H2:J2"/>
-    <mergeCell ref="E21:E29"/>
+    <mergeCell ref="E22:E30"/>
     <mergeCell ref="G11:H11"/>
-    <mergeCell ref="E1:E16"/>
+    <mergeCell ref="E1:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Made keycaps taller (for clearance)
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -879,7 +879,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -915,7 +915,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="3">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>0</v>
@@ -935,7 +935,7 @@
         <v>71</v>
       </c>
       <c r="B3" s="3">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Made a working iPart setup
Researched into iParts more and found ways to get a single base-keycap
file. I will need to restructure the project in future and update the
conventions document.

Also restructured the base-model directory (cleaner now).

I guess we're using iParts after all (thanks TFI!).
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="65">
   <si>
     <t>mm</t>
   </si>
@@ -35,12 +35,6 @@
   </si>
   <si>
     <t>k_width</t>
-  </si>
-  <si>
-    <t>k_taper1</t>
-  </si>
-  <si>
-    <t>k_taper2</t>
   </si>
   <si>
     <t>k_radius</t>
@@ -159,9 +153,6 @@
     <t>Keyswitch Pole Base Height</t>
   </si>
   <si>
-    <t>Keyboard Dimensions</t>
-  </si>
-  <si>
     <t>b_pad</t>
   </si>
   <si>
@@ -243,8 +234,23 @@
     <t>Row 1 - 2 Offset</t>
   </si>
   <si>
+    <t>Thumb row keycap height</t>
+  </si>
+  <si>
+    <t>k_taper_wide</t>
+  </si>
+  <si>
+    <t>k_taper_thin</t>
+  </si>
+  <si>
+    <t>Taper Length for keycap, where fingers won't be positioned</t>
+  </si>
+  <si>
+    <t>Taper Length for where finger goes</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Keycap pole offset for alignment </t>
+      <t xml:space="preserve">Keycap pole offset for absolute alignment </t>
     </r>
     <r>
       <rPr>
@@ -271,40 +277,35 @@
     </r>
   </si>
   <si>
-    <t>k_staper</t>
-  </si>
-  <si>
-    <t>k_ltaper</t>
-  </si>
-  <si>
-    <t>Taper Length for smaller keycap, around Left, Top and Right edges</t>
-  </si>
-  <si>
-    <t>Taper Length for larger keycap, around Left, Top and Right edges</t>
-  </si>
-  <si>
-    <t>k_sradius</t>
-  </si>
-  <si>
-    <t>k_lradius</t>
-  </si>
-  <si>
-    <t>Radius for smaller keycap along top edge</t>
-  </si>
-  <si>
-    <t>Radius for larger keycap along top edge</t>
-  </si>
-  <si>
-    <t>Taper Length for Front of keycap - where finger goes (sides, for thumb keycap)</t>
-  </si>
-  <si>
-    <t>Taper Length for keycap, around Left, Top and Right edges (top and bottom, for thumb keycap)</t>
-  </si>
-  <si>
-    <t>k_height_t</t>
-  </si>
-  <si>
-    <t>Thumb row keycap height</t>
+    <t>k_height_low</t>
+  </si>
+  <si>
+    <r>
+      <t>Key</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>oard Dimensions</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -876,10 +877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B30" sqref="B1:B30"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -907,7 +908,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -925,14 +926,14 @@
       </c>
       <c r="E2" s="17"/>
       <c r="H2" s="15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I2" s="15"/>
       <c r="J2" s="15"/>
     </row>
     <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B3" s="3">
         <v>16</v>
@@ -941,22 +942,22 @@
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="E3" s="17"/>
       <c r="H3" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I3" s="10">
         <v>1.5</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="B4" s="3">
         <v>1.5</v>
@@ -965,22 +966,22 @@
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E4" s="17"/>
       <c r="H4" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I4" s="3">
         <v>1.75</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="B5" s="3">
         <v>0.5</v>
@@ -989,70 +990,70 @@
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E5" s="17"/>
       <c r="H5" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I5" s="3">
         <v>2.25</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>61</v>
+        <v>7</v>
       </c>
       <c r="B6" s="3">
+        <v>6</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="E6" s="17"/>
       <c r="H6" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I6" s="3">
         <v>2.75</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>65</v>
+        <v>8</v>
       </c>
       <c r="B7" s="3">
-        <v>4</v>
+        <v>1.5</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>67</v>
+        <v>2</v>
       </c>
       <c r="E7" s="17"/>
       <c r="H7" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I7" s="3">
         <v>1.25</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>62</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3">
         <v>1.5</v>
@@ -1061,32 +1062,31 @@
         <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
       <c r="E8" s="17"/>
       <c r="H8" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I8" s="3">
         <v>6.5</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="4">
-        <f>B10</f>
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="B9" s="3">
+        <v>5</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="E9" s="17"/>
       <c r="J9" s="9"/>
@@ -1094,39 +1094,40 @@
     </row>
     <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3">
-        <v>6</v>
+        <v>13</v>
+      </c>
+      <c r="B10" s="4">
+        <f>$I$11/2</f>
+        <v>2.2625000000000011</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="E10" s="17"/>
     </row>
     <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B11" s="3">
-        <v>1.5</v>
+        <v>5.54</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E11" s="17"/>
       <c r="G11" s="19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H11" s="20"/>
       <c r="I11" s="10">
-        <f>B24-B23</f>
+        <f>B22-B21</f>
         <v>4.5250000000000021</v>
       </c>
       <c r="J11" s="11" t="s">
@@ -1135,309 +1136,248 @@
     </row>
     <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B12" s="3">
-        <v>1.5</v>
+        <v>1.35</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E12" s="17"/>
     </row>
-    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B13" s="3">
-        <v>5</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E13" s="17"/>
     </row>
-    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="4">
-        <f>$I$11/2</f>
-        <v>2.2625000000000011</v>
+        <v>22</v>
+      </c>
+      <c r="B14" s="3">
+        <v>15.6</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E14" s="17"/>
+        <v>23</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B15" s="3">
-        <v>5.54</v>
+        <v>3.6</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="17"/>
+        <v>25</v>
+      </c>
+      <c r="E15" s="13"/>
     </row>
     <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B16" s="3">
-        <v>1.35</v>
+        <v>5.5</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="17"/>
+        <v>28</v>
+      </c>
+      <c r="E16" s="13"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B17" s="3">
-        <v>4.4000000000000004</v>
+        <v>7</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="18"/>
+        <v>29</v>
+      </c>
+      <c r="E17" s="14"/>
     </row>
     <row r="18" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="B18" s="3">
-        <v>15.6</v>
+        <f>$B$20 +2*($B$21+$B$20)+12*($B$1+$B$20)</f>
+        <v>286.5</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>23</v>
+        <v>54</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="B19" s="3">
-        <v>3.6</v>
+        <f>$B$20+4*($B$1+$B$20)</f>
+        <v>77.400000000000006</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="13"/>
+        <v>55</v>
+      </c>
+      <c r="E19" s="17"/>
     </row>
     <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B20" s="3">
-        <v>5.5</v>
+        <v>1</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" s="13"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="E20" s="17"/>
+    </row>
+    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B21" s="3">
-        <v>7</v>
+        <f>I3*$B$1</f>
+        <v>27.150000000000002</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21" s="14"/>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="E21" s="17"/>
+    </row>
+    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B22" s="3">
-        <v>1</v>
+        <f>I4*$B$1</f>
+        <v>31.675000000000004</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>32</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="E22" s="17"/>
     </row>
     <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B23" s="3">
-        <f>I3*$B$1</f>
-        <v>27.150000000000002</v>
+        <f>I5*$B$1</f>
+        <v>40.725000000000001</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E23" s="17"/>
     </row>
     <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="3">
-        <f>I4*$B$1</f>
-        <v>31.675000000000004</v>
+        <f>I6*$B$1</f>
+        <v>49.775000000000006</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E24" s="17"/>
     </row>
     <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="3">
-        <f>I5*$B$1</f>
-        <v>40.725000000000001</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E25" s="17"/>
-    </row>
-    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" s="3">
-        <f>I6*$B$1</f>
-        <v>49.775000000000006</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E26" s="17"/>
-    </row>
-    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="3">
         <f>I7*$B$1</f>
         <v>22.625</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E27" s="17"/>
-    </row>
-    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B28" s="3">
+      <c r="C25" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25" s="17"/>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="3">
         <f>I8*$B$1</f>
         <v>117.65</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E28" s="17"/>
-    </row>
-    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" s="3">
-        <f>$B$22 +2*($B$23+$B$22)+12*($B$1+$B$22)</f>
-        <v>286.5</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E29" s="17"/>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B30" s="3">
-        <f>$B$22+4*($B$1+$B$22)</f>
-        <v>77.400000000000006</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E30" s="18"/>
+      <c r="C26" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="E14:E17"/>
     <mergeCell ref="H2:J2"/>
-    <mergeCell ref="E22:E30"/>
+    <mergeCell ref="E18:E26"/>
     <mergeCell ref="G11:H11"/>
-    <mergeCell ref="E1:E17"/>
+    <mergeCell ref="E1:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added 0.25mm clearance on CMX pole
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="67">
   <si>
     <t>mm</t>
   </si>
@@ -61,9 +61,6 @@
     <t>k_cmxw</t>
   </si>
   <si>
-    <t>Keycap pole Cherry MX Width (for joint)</t>
-  </si>
-  <si>
     <t>k_poledia</t>
   </si>
   <si>
@@ -71,9 +68,6 @@
   </si>
   <si>
     <t>k_cmxl</t>
-  </si>
-  <si>
-    <t>Keycap pole Cherry MX Length (for joint)</t>
   </si>
   <si>
     <r>
@@ -306,6 +300,18 @@
       </rPr>
       <t>oard Dimensions</t>
     </r>
+  </si>
+  <si>
+    <t>CLEARANCE</t>
+  </si>
+  <si>
+    <t>Hole clearance (on all sides)</t>
+  </si>
+  <si>
+    <t>Keycap pole Cherry MX Width (for joint / base of the pole)</t>
+  </si>
+  <si>
+    <t>Keycap pole Cherry MX Length (for joint / base of the pole)</t>
   </si>
 </sst>
 </file>
@@ -516,7 +522,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -571,6 +577,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -880,7 +892,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -908,7 +920,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -926,14 +938,14 @@
       </c>
       <c r="E2" s="17"/>
       <c r="H2" s="15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I2" s="15"/>
       <c r="J2" s="15"/>
     </row>
     <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B3" s="3">
         <v>16</v>
@@ -942,22 +954,22 @@
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E3" s="17"/>
       <c r="H3" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I3" s="10">
         <v>1.5</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B4" s="3">
         <v>1.5</v>
@@ -966,22 +978,22 @@
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E4" s="17"/>
       <c r="H4" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I4" s="3">
         <v>1.75</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B5" s="3">
         <v>0.5</v>
@@ -990,17 +1002,17 @@
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E5" s="17"/>
       <c r="H5" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I5" s="3">
         <v>2.25</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -1018,13 +1030,13 @@
       </c>
       <c r="E6" s="17"/>
       <c r="H6" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I6" s="3">
         <v>2.75</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -1042,13 +1054,13 @@
       </c>
       <c r="E7" s="17"/>
       <c r="H7" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I7" s="3">
         <v>1.25</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -1066,13 +1078,13 @@
       </c>
       <c r="E8" s="17"/>
       <c r="H8" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I8" s="3">
         <v>6.5</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -1104,13 +1116,13 @@
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E10" s="17"/>
     </row>
     <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="3">
         <v>5.54</v>
@@ -1119,11 +1131,11 @@
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E11" s="17"/>
       <c r="G11" s="19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H11" s="20"/>
       <c r="I11" s="10">
@@ -1139,34 +1151,36 @@
         <v>14</v>
       </c>
       <c r="B12" s="3">
-        <v>1.35</v>
+        <f>1.35 + $I$16</f>
+        <v>1.6</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="E12" s="17"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="3">
-        <v>4.4000000000000004</v>
+        <f>4.1 + $I$16</f>
+        <v>4.3499999999999996</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="E13" s="17"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B14" s="3">
         <v>15.6</v>
@@ -1175,15 +1189,20 @@
         <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>21</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
     </row>
     <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B15" s="3">
         <v>3.6</v>
@@ -1192,13 +1211,16 @@
         <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E15" s="13"/>
+      <c r="H15" s="22" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B16" s="3">
         <v>5.5</v>
@@ -1207,13 +1229,20 @@
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E16" s="13"/>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H16" s="22"/>
+      <c r="I16" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B17" s="3">
         <v>7</v>
@@ -1222,13 +1251,14 @@
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E17" s="14"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="H17" s="22"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B18" s="3">
         <f>$B$20 +2*($B$21+$B$20)+12*($B$1+$B$20)</f>
@@ -1238,15 +1268,15 @@
         <v>0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B19" s="3">
         <f>$B$20+4*($B$1+$B$20)</f>
@@ -1256,13 +1286,13 @@
         <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E19" s="17"/>
     </row>
-    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B20" s="3">
         <v>1</v>
@@ -1271,113 +1301,115 @@
         <v>0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E20" s="17"/>
     </row>
-    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="3">
+        <f t="shared" ref="B21:B26" si="0">I3*$B$1</f>
+        <v>27.150000000000002</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="17"/>
+    </row>
+    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="3">
-        <f>I3*$B$1</f>
-        <v>27.150000000000002</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D21" s="2" t="s">
+      <c r="B22" s="3">
+        <f t="shared" si="0"/>
+        <v>31.675000000000004</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="17"/>
+    </row>
+    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="3">
+        <f t="shared" si="0"/>
+        <v>40.725000000000001</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" s="17"/>
+    </row>
+    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="3">
+        <f t="shared" si="0"/>
+        <v>49.775000000000006</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" s="17"/>
+    </row>
+    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="3">
+        <f t="shared" si="0"/>
+        <v>22.625</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E21" s="17"/>
-    </row>
-    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="3">
-        <f>I4*$B$1</f>
-        <v>31.675000000000004</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="E25" s="17"/>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="3">
+        <f t="shared" si="0"/>
+        <v>117.65</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="17"/>
-    </row>
-    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="3">
-        <f>I5*$B$1</f>
-        <v>40.725000000000001</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E23" s="17"/>
-    </row>
-    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="3">
-        <f>I6*$B$1</f>
-        <v>49.775000000000006</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E24" s="17"/>
-    </row>
-    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B25" s="3">
-        <f>I7*$B$1</f>
-        <v>22.625</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E25" s="17"/>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="3">
-        <f>I8*$B$1</f>
-        <v>117.65</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="E26" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
     <mergeCell ref="E14:E17"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="E18:E26"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="E1:E13"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="H15:H17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Relinked files to the parameters spreadsheet
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -892,7 +892,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -928,7 +928,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="3">
-        <v>18</v>
+        <v>16.5</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>0</v>
@@ -948,7 +948,7 @@
         <v>61</v>
       </c>
       <c r="B3" s="3">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Added pole height, shortened keycap
To prevent collisions between the keycap skirt and the keyswitch, the
actual keycap section was foreshortened. This shouldn't really change
the aesthetic of the keycaps, because they're so tall, but that's the
least of our concerns.

The wall thickness of the pole is 0.4mm too thin - we'll see if this can
be rectified without causing clearance issues with the keyswitch. If
not, we may need to print forks instead of a pole - which will be
equally interesting.

Also, found a bug in Inventor that meant I had to set the capOffset of
the thumb variant to 0.001 instead of 0 - otherwise, direction was not
preserved (a big problem).
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="69">
   <si>
     <t>mm</t>
   </si>
@@ -312,6 +312,12 @@
   </si>
   <si>
     <t>Keycap pole Cherry MX Length (for joint / base of the pole)</t>
+  </si>
+  <si>
+    <t>k_shortening</t>
+  </si>
+  <si>
+    <t>The amount that the pole sticks out from the bottom of the keycap</t>
   </si>
 </sst>
 </file>
@@ -889,10 +895,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -1139,7 +1145,7 @@
       </c>
       <c r="H11" s="20"/>
       <c r="I11" s="10">
-        <f>B22-B21</f>
+        <f>B23-B22</f>
         <v>4.5250000000000021</v>
       </c>
       <c r="J11" s="11" t="s">
@@ -1162,7 +1168,7 @@
       </c>
       <c r="E12" s="17"/>
     </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -1178,58 +1184,58 @@
       </c>
       <c r="E13" s="17"/>
     </row>
-    <row r="14" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="B14" s="3">
-        <v>15.6</v>
+        <v>4.5</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>19</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="E14" s="18"/>
       <c r="H14" s="21" t="s">
         <v>63</v>
       </c>
       <c r="I14" s="21"/>
       <c r="J14" s="21"/>
     </row>
-    <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B15" s="3">
-        <v>3.6</v>
+        <v>15.6</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="13"/>
+        <v>21</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>19</v>
+      </c>
       <c r="H15" s="22" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B16" s="3">
-        <v>5.5</v>
+        <v>3.6</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E16" s="13"/>
       <c r="H16" s="22"/>
@@ -1240,176 +1246,191 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="13"/>
+      <c r="H17" s="22"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B18" s="3">
         <v>7</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="C18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="14"/>
-      <c r="H17" s="22"/>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="E18" s="14"/>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="3">
-        <f>$B$20 +2*($B$21+$B$20)+12*($B$1+$B$20)</f>
+      <c r="B19" s="3">
+        <f>$B$21 +2*($B$22+$B$21)+12*($B$1+$B$21)</f>
         <v>286.5</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D18" s="2" t="s">
+      <c r="C19" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E19" s="16" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" s="3">
-        <f>$B$20+4*($B$1+$B$20)</f>
-        <v>77.400000000000006</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" s="17"/>
     </row>
     <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="B20" s="3">
-        <v>1</v>
+        <f>$B$21+4*($B$1+$B$21)</f>
+        <v>77.400000000000006</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="E20" s="17"/>
     </row>
     <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B21" s="3">
-        <f t="shared" ref="B21:B26" si="0">I3*$B$1</f>
-        <v>27.150000000000002</v>
+        <v>1</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="E21" s="17"/>
     </row>
     <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B22" s="3">
-        <f t="shared" si="0"/>
-        <v>31.675000000000004</v>
+        <f>I3*$B$1</f>
+        <v>27.150000000000002</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E22" s="17"/>
     </row>
     <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" s="3">
-        <f t="shared" si="0"/>
-        <v>40.725000000000001</v>
+        <f>I4*$B$1</f>
+        <v>31.675000000000004</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E23" s="17"/>
     </row>
     <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" s="3">
-        <f t="shared" si="0"/>
-        <v>49.775000000000006</v>
+        <f>I5*$B$1</f>
+        <v>40.725000000000001</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E24" s="17"/>
     </row>
     <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="3">
+        <f>I6*$B$1</f>
+        <v>49.775000000000006</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="17"/>
+    </row>
+    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="3">
-        <f t="shared" si="0"/>
+      <c r="B26" s="3">
+        <f>I7*$B$1</f>
         <v>22.625</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D25" s="2" t="s">
+      <c r="C26" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E25" s="17"/>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+      <c r="E26" s="17"/>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="3">
-        <f t="shared" si="0"/>
+      <c r="B27" s="3">
+        <f>I8*$B$1</f>
         <v>117.65</v>
       </c>
-      <c r="C26" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D26" s="2" t="s">
+      <c r="C27" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E26" s="18"/>
+      <c r="E27" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="E15:E18"/>
     <mergeCell ref="H2:J2"/>
-    <mergeCell ref="E18:E26"/>
+    <mergeCell ref="E19:E27"/>
     <mergeCell ref="G11:H11"/>
-    <mergeCell ref="E1:E13"/>
     <mergeCell ref="H14:J14"/>
     <mergeCell ref="H15:H17"/>
+    <mergeCell ref="E1:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Decreased the cut-in depth to improve strength of part
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="71">
   <si>
     <t>mm</t>
   </si>
@@ -318,6 +318,37 @@
   </si>
   <si>
     <t>The amount that the pole sticks out from the bottom of the keycap</t>
+  </si>
+  <si>
+    <t>k_cmxd</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Keycap Cherry MX Cut in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>depth</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Keep it as low as possible for strength reasons.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -895,10 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -1145,7 +1176,7 @@
       </c>
       <c r="H11" s="20"/>
       <c r="I11" s="10">
-        <f>B23-B22</f>
+        <f>B24-B23</f>
         <v>4.5250000000000021</v>
       </c>
       <c r="J11" s="11" t="s">
@@ -1184,60 +1215,60 @@
       </c>
       <c r="E13" s="17"/>
     </row>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B14" s="3">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" s="18"/>
+        <v>70</v>
+      </c>
+      <c r="E14" s="17"/>
       <c r="H14" s="21" t="s">
         <v>63</v>
       </c>
       <c r="I14" s="21"/>
       <c r="J14" s="21"/>
     </row>
-    <row r="15" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="B15" s="3">
-        <v>15.6</v>
+        <v>4.5</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>19</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="E15" s="18"/>
       <c r="H15" s="22" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B16" s="3">
-        <v>3.6</v>
+        <v>15.6</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="13"/>
+        <v>21</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>19</v>
+      </c>
       <c r="H16" s="22"/>
       <c r="I16" s="3">
         <v>0.25</v>
@@ -1248,189 +1279,204 @@
     </row>
     <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17" s="3">
-        <v>5.5</v>
+        <v>3.6</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E17" s="13"/>
       <c r="H17" s="22"/>
     </row>
-    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="13"/>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B19" s="3">
         <v>7</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D18" s="2" t="s">
+      <c r="C19" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="14"/>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="E19" s="14"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="3">
-        <f>$B$21 +2*($B$22+$B$21)+12*($B$1+$B$21)</f>
+      <c r="B20" s="3">
+        <f>$B$22 +2*($B$23+$B$22)+12*($B$1+$B$22)</f>
         <v>286.5</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="2" t="s">
+      <c r="C20" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="E20" s="16" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" s="3">
-        <f>$B$21+4*($B$1+$B$21)</f>
-        <v>77.400000000000006</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20" s="17"/>
     </row>
     <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="B21" s="3">
-        <v>1</v>
+        <f>$B$22+4*($B$1+$B$22)</f>
+        <v>77.400000000000006</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="E21" s="17"/>
     </row>
     <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="3">
+        <v>1</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="17"/>
+    </row>
+    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B23" s="3">
         <f>I3*$B$1</f>
         <v>27.150000000000002</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="C23" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E22" s="17"/>
-    </row>
-    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="E23" s="17"/>
+    </row>
+    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B24" s="3">
         <f>I4*$B$1</f>
         <v>31.675000000000004</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="C24" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="17"/>
-    </row>
-    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="E24" s="17"/>
+    </row>
+    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B25" s="3">
         <f>I5*$B$1</f>
         <v>40.725000000000001</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="C25" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E24" s="17"/>
-    </row>
-    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="E25" s="17"/>
+    </row>
+    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B26" s="3">
         <f>I6*$B$1</f>
         <v>49.775000000000006</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D25" s="2" t="s">
+      <c r="C26" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E25" s="17"/>
-    </row>
-    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="E26" s="17"/>
+    </row>
+    <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B27" s="3">
         <f>I7*$B$1</f>
         <v>22.625</v>
       </c>
-      <c r="C26" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D26" s="2" t="s">
+      <c r="C27" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E26" s="17"/>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+      <c r="E27" s="17"/>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B28" s="3">
         <f>I8*$B$1</f>
         <v>117.65</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D27" s="2" t="s">
+      <c r="C28" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E27" s="18"/>
+      <c r="E28" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="E15:E18"/>
+    <mergeCell ref="E16:E19"/>
     <mergeCell ref="H2:J2"/>
-    <mergeCell ref="E19:E27"/>
+    <mergeCell ref="E20:E28"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="H14:J14"/>
     <mergeCell ref="H15:H17"/>
-    <mergeCell ref="E1:E14"/>
+    <mergeCell ref="E1:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated styling on param spreadsheet
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="72">
   <si>
     <t>mm</t>
   </si>
@@ -349,6 +349,9 @@
       </rPr>
       <t xml:space="preserve"> Keep it as low as possible for strength reasons.</t>
     </r>
+  </si>
+  <si>
+    <t>Varies depending on 3D printer</t>
   </si>
 </sst>
 </file>
@@ -559,7 +562,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -620,6 +623,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -929,7 +935,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="H18" sqref="H18:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -1257,7 +1263,7 @@
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="23">
         <v>15.6</v>
       </c>
       <c r="C16" s="5" t="s">
@@ -1307,6 +1313,9 @@
         <v>26</v>
       </c>
       <c r="E18" s="13"/>
+      <c r="H18" s="22" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
@@ -1322,12 +1331,13 @@
         <v>27</v>
       </c>
       <c r="E19" s="14"/>
+      <c r="H19" s="22"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="4">
         <f>$B$22 +2*($B$23+$B$22)+12*($B$1+$B$22)</f>
         <v>286.5</v>
       </c>
@@ -1340,12 +1350,13 @@
       <c r="E20" s="16" t="s">
         <v>62</v>
       </c>
+      <c r="H20" s="22"/>
     </row>
     <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="4">
         <f>$B$22+4*($B$1+$B$22)</f>
         <v>77.400000000000006</v>
       </c>
@@ -1376,8 +1387,8 @@
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="3">
-        <f>I3*$B$1</f>
+      <c r="B23" s="4">
+        <f t="shared" ref="B23:B28" si="0">I3*$B$1</f>
         <v>27.150000000000002</v>
       </c>
       <c r="C23" s="5" t="s">
@@ -1392,8 +1403,8 @@
       <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="3">
-        <f>I4*$B$1</f>
+      <c r="B24" s="4">
+        <f t="shared" si="0"/>
         <v>31.675000000000004</v>
       </c>
       <c r="C24" s="5" t="s">
@@ -1408,8 +1419,8 @@
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="3">
-        <f>I5*$B$1</f>
+      <c r="B25" s="4">
+        <f t="shared" si="0"/>
         <v>40.725000000000001</v>
       </c>
       <c r="C25" s="5" t="s">
@@ -1424,8 +1435,8 @@
       <c r="A26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="3">
-        <f>I6*$B$1</f>
+      <c r="B26" s="4">
+        <f t="shared" si="0"/>
         <v>49.775000000000006</v>
       </c>
       <c r="C26" s="5" t="s">
@@ -1440,8 +1451,8 @@
       <c r="A27" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="3">
-        <f>I7*$B$1</f>
+      <c r="B27" s="4">
+        <f t="shared" si="0"/>
         <v>22.625</v>
       </c>
       <c r="C27" s="5" t="s">
@@ -1456,8 +1467,8 @@
       <c r="A28" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="3">
-        <f>I8*$B$1</f>
+      <c r="B28" s="4">
+        <f t="shared" si="0"/>
         <v>117.65</v>
       </c>
       <c r="C28" s="5" t="s">
@@ -1469,7 +1480,7 @@
       <c r="E28" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="E16:E19"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="E20:E28"/>
@@ -1477,6 +1488,7 @@
     <mergeCell ref="H14:J14"/>
     <mergeCell ref="H15:H17"/>
     <mergeCell ref="E1:E15"/>
+    <mergeCell ref="H18:H20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Verified Dimensions against physical switches
Very slight adjustments were made to the dimensions that I believe will
improve the fit of the keycap to the switch. Also, the cut-in depth was
reduced, which will increase the strength with marginal extra print
time.

The project is almost complete - all that's left is to do test prints
and mark it off as finished!
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="120" yWindow="90" windowWidth="28635" windowHeight="13215"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Keycap Dimensions" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -144,9 +144,6 @@
     <t>Keyswitch Pole Base Width</t>
   </si>
   <si>
-    <t>Keyswitch Pole Base Height</t>
-  </si>
-  <si>
     <t>b_pad</t>
   </si>
   <si>
@@ -352,6 +349,9 @@
   </si>
   <si>
     <t>Varies depending on 3D printer</t>
+  </si>
+  <si>
+    <t>Keyswitch Pole Base Length</t>
   </si>
 </sst>
 </file>
@@ -591,6 +591,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -623,9 +626,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -935,7 +935,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18:H20"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -954,7 +954,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="3">
-        <v>18.100000000000001</v>
+        <v>18.2</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>0</v>
@@ -962,7 +962,7 @@
       <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="17" t="s">
         <v>18</v>
       </c>
     </row>
@@ -979,16 +979,16 @@
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="H2" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
+      <c r="E2" s="18"/>
+      <c r="H2" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
     </row>
     <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="3">
         <v>15</v>
@@ -997,22 +997,22 @@
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="17"/>
+        <v>54</v>
+      </c>
+      <c r="E3" s="18"/>
       <c r="H3" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I3" s="10">
         <v>1.5</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" s="3">
         <v>1.5</v>
@@ -1021,22 +1021,22 @@
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4" s="17"/>
+        <v>57</v>
+      </c>
+      <c r="E4" s="18"/>
       <c r="H4" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I4" s="3">
         <v>1.75</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="3">
         <v>0.5</v>
@@ -1045,17 +1045,17 @@
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="17"/>
+        <v>58</v>
+      </c>
+      <c r="E5" s="18"/>
       <c r="H5" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I5" s="3">
         <v>2.25</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -1071,15 +1071,15 @@
       <c r="D6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="17"/>
+      <c r="E6" s="18"/>
       <c r="H6" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I6" s="3">
         <v>2.75</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -1095,15 +1095,15 @@
       <c r="D7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="17"/>
+      <c r="E7" s="18"/>
       <c r="H7" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I7" s="3">
         <v>1.25</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -1119,15 +1119,15 @@
       <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="17"/>
+      <c r="E8" s="18"/>
       <c r="H8" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I8" s="3">
         <v>6.5</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -1143,7 +1143,7 @@
       <c r="D9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="17"/>
+      <c r="E9" s="18"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
     </row>
@@ -1153,22 +1153,22 @@
       </c>
       <c r="B10" s="4">
         <f>$I$11/2</f>
-        <v>2.2625000000000011</v>
+        <v>2.2750000000000004</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E10" s="17"/>
+        <v>59</v>
+      </c>
+      <c r="E10" s="18"/>
     </row>
     <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="3">
-        <v>5.54</v>
+        <v>5.3</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>0</v>
@@ -1176,14 +1176,14 @@
       <c r="D11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="17"/>
-      <c r="G11" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="H11" s="20"/>
+      <c r="E11" s="18"/>
+      <c r="G11" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="21"/>
       <c r="I11" s="10">
         <f>B24-B23</f>
-        <v>4.5250000000000021</v>
+        <v>4.5500000000000007</v>
       </c>
       <c r="J11" s="11" t="s">
         <v>0</v>
@@ -1194,16 +1194,16 @@
         <v>14</v>
       </c>
       <c r="B12" s="3">
-        <f>1.35 + $I$16</f>
-        <v>1.6</v>
+        <f>1.3 + $I$16</f>
+        <v>1.55</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E12" s="17"/>
+        <v>64</v>
+      </c>
+      <c r="E12" s="18"/>
     </row>
     <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -1217,33 +1217,33 @@
         <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E13" s="17"/>
+        <v>65</v>
+      </c>
+      <c r="E13" s="18"/>
     </row>
     <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="3">
+        <v>4</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="3">
-        <v>5</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E14" s="17"/>
-      <c r="H14" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
+      <c r="E14" s="18"/>
+      <c r="H14" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B15" s="3">
         <v>4.5</v>
@@ -1252,19 +1252,19 @@
         <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="18"/>
-      <c r="H15" s="22" t="s">
-        <v>64</v>
+        <v>67</v>
+      </c>
+      <c r="E15" s="19"/>
+      <c r="H15" s="23" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="23">
-        <v>15.6</v>
+      <c r="B16" s="12">
+        <v>14.4</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>0</v>
@@ -1272,10 +1272,10 @@
       <c r="D16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="H16" s="22"/>
+      <c r="H16" s="23"/>
       <c r="I16" s="3">
         <v>0.25</v>
       </c>
@@ -1296,15 +1296,15 @@
       <c r="D17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="13"/>
-      <c r="H17" s="22"/>
+      <c r="E17" s="14"/>
+      <c r="H17" s="23"/>
     </row>
     <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B18" s="3">
-        <v>5.5</v>
+        <v>5.4</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>0</v>
@@ -1312,9 +1312,9 @@
       <c r="D18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="13"/>
-      <c r="H18" s="22" t="s">
-        <v>71</v>
+      <c r="E18" s="14"/>
+      <c r="H18" s="23" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1322,55 +1322,55 @@
         <v>25</v>
       </c>
       <c r="B19" s="3">
-        <v>7</v>
+        <v>7.45</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="14"/>
-      <c r="H19" s="22"/>
+        <v>71</v>
+      </c>
+      <c r="E19" s="15"/>
+      <c r="H19" s="23"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B20" s="4">
         <f>$B$22 +2*($B$23+$B$22)+12*($B$1+$B$22)</f>
-        <v>286.5</v>
+        <v>288</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="H20" s="22"/>
+        <v>51</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="H20" s="23"/>
     </row>
     <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B21" s="4">
         <f>$B$22+4*($B$1+$B$22)</f>
-        <v>77.400000000000006</v>
+        <v>77.8</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="17"/>
+        <v>52</v>
+      </c>
+      <c r="E21" s="18"/>
     </row>
     <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="3">
         <v>1</v>
@@ -1379,105 +1379,105 @@
         <v>0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E22" s="17"/>
+        <v>28</v>
+      </c>
+      <c r="E22" s="18"/>
     </row>
     <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="4">
         <f t="shared" ref="B23:B28" si="0">I3*$B$1</f>
-        <v>27.150000000000002</v>
+        <v>27.299999999999997</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" s="17"/>
+        <v>46</v>
+      </c>
+      <c r="E23" s="18"/>
     </row>
     <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" s="4">
         <f t="shared" si="0"/>
-        <v>31.675000000000004</v>
+        <v>31.849999999999998</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E24" s="17"/>
+        <v>43</v>
+      </c>
+      <c r="E24" s="18"/>
     </row>
     <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" s="4">
         <f t="shared" si="0"/>
-        <v>40.725000000000001</v>
+        <v>40.949999999999996</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E25" s="17"/>
+        <v>47</v>
+      </c>
+      <c r="E25" s="18"/>
     </row>
     <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26" s="4">
         <f t="shared" si="0"/>
-        <v>49.775000000000006</v>
+        <v>50.05</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E26" s="17"/>
+        <v>44</v>
+      </c>
+      <c r="E26" s="18"/>
     </row>
     <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B27" s="4">
         <f t="shared" si="0"/>
-        <v>22.625</v>
+        <v>22.75</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E27" s="17"/>
+        <v>48</v>
+      </c>
+      <c r="E27" s="18"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B28" s="4">
         <f t="shared" si="0"/>
-        <v>117.65</v>
+        <v>118.3</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E28" s="18"/>
+        <v>45</v>
+      </c>
+      <c r="E28" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>